<commit_message>
Work on the compatibility issues with Linux
</commit_message>
<xml_diff>
--- a/dev_info/gk_linux_mono_compatibility_ru.xlsx
+++ b/dev_info/gk_linux_mono_compatibility_ru.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="139">
   <si>
     <t>Базовый функционал</t>
   </si>
@@ -264,9 +264,6 @@
     <t>Отправка логов почтой</t>
   </si>
   <si>
-    <t>MAPI недоступен</t>
-  </si>
-  <si>
     <t>Странный скроллинг и отображение</t>
   </si>
   <si>
@@ -384,9 +381,6 @@
     <t>Функционал</t>
   </si>
   <si>
-    <t>Неправильное расположение закладок</t>
-  </si>
-  <si>
     <t>Съехал интерфейс, кнопки недоступны</t>
   </si>
   <si>
@@ -399,27 +393,15 @@
     <t>Просмотр графа связей</t>
   </si>
   <si>
-    <t>Работает везде, кроме главного меню; нельзя получить код текущего языка</t>
-  </si>
-  <si>
     <t>SingleInstance не работает (Main)</t>
   </si>
   <si>
     <t>1.31</t>
   </si>
   <si>
-    <t>Искажение размера окна; не отображается при частом обновлении</t>
-  </si>
-  <si>
     <t>Иконки основного тулбара</t>
   </si>
   <si>
-    <t>ArborGVT зависает</t>
-  </si>
-  <si>
-    <t>Часть кнопок теряет прозрачность</t>
-  </si>
-  <si>
     <t>Не доступен OpenGL, dll-depend</t>
   </si>
   <si>
@@ -439,6 +421,18 @@
   </si>
   <si>
     <t>Не работает позиционирование в списке; иногда список теряет фокус (?!!!)</t>
+  </si>
+  <si>
+    <t>Не отображается при частом обновлении</t>
+  </si>
+  <si>
+    <t>Не работает получение кода текущего языка (но работает всё остальное)</t>
+  </si>
+  <si>
+    <t>Неправильное расположение закладок и сбой автомасштаба (персональный фильтр)</t>
+  </si>
+  <si>
+    <t>ArborGVT подвисает</t>
   </si>
 </sst>
 </file>
@@ -470,7 +464,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -507,6 +501,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -535,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
@@ -564,6 +564,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -870,31 +873,31 @@
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="55.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="71.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="81.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>121</v>
-      </c>
       <c r="C1" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -904,7 +907,7 @@
       <c r="C2" s="11"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -916,7 +919,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -927,10 +930,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -942,21 +945,19 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="13">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C6" s="12">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -968,7 +969,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -980,7 +981,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -992,7 +993,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -1004,7 +1005,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1016,7 +1017,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1028,7 +1029,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -1040,7 +1041,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -1051,10 +1052,10 @@
         <v>0.75</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -1066,7 +1067,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -1074,13 +1075,13 @@
         <v>47</v>
       </c>
       <c r="C16" s="14">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -1088,13 +1089,13 @@
         <v>48</v>
       </c>
       <c r="C17" s="14">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1108,7 +1109,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -1120,7 +1121,7 @@
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -1131,10 +1132,10 @@
         <v>0.5</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -1145,10 +1146,10 @@
         <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>50</v>
       </c>
@@ -1159,10 +1160,10 @@
         <v>0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>51</v>
       </c>
@@ -1174,7 +1175,7 @@
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
@@ -1186,7 +1187,7 @@
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>53</v>
       </c>
@@ -1200,7 +1201,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>54</v>
       </c>
@@ -1211,10 +1212,10 @@
         <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>55</v>
       </c>
@@ -1226,7 +1227,7 @@
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>56</v>
       </c>
@@ -1238,7 +1239,7 @@
       </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>57</v>
       </c>
@@ -1250,7 +1251,7 @@
       </c>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
@@ -1262,7 +1263,7 @@
       </c>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>59</v>
       </c>
@@ -1272,21 +1273,21 @@
       <c r="C31" s="15"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="14">
-        <v>0.75</v>
+      <c r="C32" s="16">
+        <v>0.9</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>61</v>
       </c>
@@ -1298,43 +1299,41 @@
       </c>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C34" s="14">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C35" s="13">
-        <v>0</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+      <c r="C35" s="12">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="15"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>27</v>
       </c>
@@ -1344,7 +1343,7 @@
       <c r="C37" s="11"/>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>45</v>
       </c>
@@ -1356,125 +1355,127 @@
       </c>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="12">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C39" s="12">
-        <v>1</v>
-      </c>
-      <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+      <c r="C40" s="12">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C40" s="15"/>
-      <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="C41" s="12">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C41" s="12">
-        <v>1</v>
-      </c>
-      <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+      <c r="C42" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C42" s="13">
-        <v>0</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="C43" s="12">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44" s="12">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C43" s="12">
-        <v>1</v>
-      </c>
-      <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B44" s="1" t="s">
+      <c r="C45" s="12">
+        <v>1</v>
+      </c>
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C44" s="12">
-        <v>1</v>
-      </c>
-      <c r="D44" s="1"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C45" s="12">
-        <v>1</v>
-      </c>
-      <c r="D45" s="1"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C46" s="13">
-        <v>0</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="C47" s="12">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C47" s="12">
-        <v>1</v>
-      </c>
-      <c r="D47" s="1"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="15"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>29</v>
       </c>
@@ -1484,97 +1485,109 @@
       <c r="C49" s="11"/>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C50" s="14">
+        <v>85</v>
+      </c>
+      <c r="C50" s="16">
         <v>0.9</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C51" s="12"/>
+        <v>86</v>
+      </c>
+      <c r="C51" s="12">
+        <v>1</v>
+      </c>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C52" s="12"/>
+        <v>87</v>
+      </c>
+      <c r="C52" s="12">
+        <v>1</v>
+      </c>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C53" s="12"/>
+        <v>91</v>
+      </c>
+      <c r="C53" s="12">
+        <v>1</v>
+      </c>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C54" s="12"/>
+        <v>92</v>
+      </c>
+      <c r="C54" s="12">
+        <v>1</v>
+      </c>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C55" s="12"/>
+        <v>93</v>
+      </c>
+      <c r="C55" s="12">
+        <v>1</v>
+      </c>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C56" s="13">
         <v>0</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" s="12">
+        <v>1</v>
+      </c>
+      <c r="D57" s="1"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C57" s="12"/>
-      <c r="D57" s="1"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>38</v>
@@ -1583,55 +1596,57 @@
         <v>0</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" s="12">
+        <v>1</v>
+      </c>
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C59" s="12"/>
-      <c r="D59" s="1"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="B60" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C60" s="13">
         <v>0</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="15"/>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="15"/>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="8"/>
       <c r="C63" s="10">
         <f>AVERAGE(C2:C62)</f>
-        <v>0.68666666666666665</v>
+        <v>0.81698113207547163</v>
       </c>
       <c r="D63" s="8"/>
     </row>
@@ -1651,7 +1666,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1663,7 +1678,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Linux-projects, and small fixes problems
</commit_message>
<xml_diff>
--- a/dev_info/gk_linux_mono_compatibility_ru.xlsx
+++ b/dev_info/gk_linux_mono_compatibility_ru.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="138">
   <si>
     <t>Базовый функционал</t>
   </si>
@@ -424,9 +424,6 @@
   </si>
   <si>
     <t>Не отображается при частом обновлении</t>
-  </si>
-  <si>
-    <t>Не работает получение кода текущего языка (но работает всё остальное)</t>
   </si>
   <si>
     <t>Неправильное расположение закладок и сбой автомасштаба (персональный фильтр)</t>
@@ -872,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,7 +1089,7 @@
         <v>0.75</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1270,7 +1267,9 @@
       <c r="B31" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="15"/>
+      <c r="C31" s="12">
+        <v>1</v>
+      </c>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1280,12 +1279,10 @@
       <c r="B32" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>136</v>
-      </c>
+      <c r="C32" s="12">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -1452,7 +1449,7 @@
         <v>0.75</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1646,7 +1643,7 @@
       <c r="B63" s="8"/>
       <c r="C63" s="10">
         <f>AVERAGE(C2:C62)</f>
-        <v>0.81698113207547163</v>
+        <v>0.82222222222222219</v>
       </c>
       <c r="D63" s="8"/>
     </row>

</xml_diff>

<commit_message>
Bug fixes when running in Mono: - no render progression in the rapid functions; - loss of focus of the main list in quick search; - no scrolling on an invisible point in a quick search; - the failure of the autoscaling control for merge records; - the failure of the scaling of the dialog for main filtering.
</commit_message>
<xml_diff>
--- a/dev_info/gk_linux_mono_compatibility_ru.xlsx
+++ b/dev_info/gk_linux_mono_compatibility_ru.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="134">
   <si>
     <t>Базовый функционал</t>
   </si>
@@ -381,9 +381,6 @@
     <t>Функционал</t>
   </si>
   <si>
-    <t>Съехал интерфейс, кнопки недоступны</t>
-  </si>
-  <si>
     <t>Прогрессия</t>
   </si>
   <si>
@@ -409,15 +406,6 @@
   </si>
   <si>
     <t>Только генерация и просмотр HTML, не формируется PDF (iTextSharp), dll-depend</t>
-  </si>
-  <si>
-    <t>Не работает позиционирование в списке; иногда список теряет фокус (?!!!)</t>
-  </si>
-  <si>
-    <t>Не отображается при частом обновлении</t>
-  </si>
-  <si>
-    <t>Неправильное расположение закладок и сбой автомасштаба (персональный фильтр)</t>
   </si>
   <si>
     <t>ArborGVT подвисает</t>
@@ -878,18 +866,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="81.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="81.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>119</v>
       </c>
@@ -903,7 +891,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -913,7 +901,7 @@
       <c r="C2" s="11"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -925,7 +913,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -936,10 +924,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -951,7 +939,7 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>80</v>
       </c>
@@ -963,7 +951,7 @@
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -975,7 +963,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -987,7 +975,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -999,7 +987,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -1011,7 +999,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1023,7 +1011,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1035,7 +1023,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -1047,7 +1035,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -1061,7 +1049,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -1073,35 +1061,31 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="14">
-        <v>0.75</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="12">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="14">
-        <v>0.75</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="12">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1115,7 +1099,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -1127,7 +1111,7 @@
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -1138,10 +1122,10 @@
         <v>0.5</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -1152,10 +1136,10 @@
         <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>50</v>
       </c>
@@ -1169,7 +1153,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>51</v>
       </c>
@@ -1181,7 +1165,7 @@
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
@@ -1193,7 +1177,7 @@
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>53</v>
       </c>
@@ -1207,7 +1191,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>54</v>
       </c>
@@ -1218,10 +1202,10 @@
         <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>55</v>
       </c>
@@ -1233,7 +1217,7 @@
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>56</v>
       </c>
@@ -1245,7 +1229,7 @@
       </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>57</v>
       </c>
@@ -1257,7 +1241,7 @@
       </c>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
@@ -1269,7 +1253,7 @@
       </c>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>59</v>
       </c>
@@ -1281,7 +1265,7 @@
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>60</v>
       </c>
@@ -1293,7 +1277,7 @@
       </c>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>61</v>
       </c>
@@ -1305,41 +1289,39 @@
       </c>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C34" s="14">
-        <v>0.75</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="C34" s="12">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C35" s="12">
         <v>1</v>
       </c>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="15"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>27</v>
       </c>
@@ -1349,7 +1331,7 @@
       <c r="C37" s="11"/>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>45</v>
       </c>
@@ -1361,7 +1343,7 @@
       </c>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>106</v>
       </c>
@@ -1373,7 +1355,7 @@
       </c>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>107</v>
       </c>
@@ -1385,7 +1367,7 @@
       </c>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>108</v>
       </c>
@@ -1397,21 +1379,19 @@
       </c>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C42" s="14">
-        <v>0.75</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="12">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>110</v>
       </c>
@@ -1423,7 +1403,7 @@
       </c>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>111</v>
       </c>
@@ -1435,33 +1415,33 @@
       </c>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C45" s="12">
         <v>1</v>
       </c>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C46" s="14">
         <v>0.75</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>114</v>
       </c>
@@ -1473,7 +1453,7 @@
       </c>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>115</v>
       </c>
@@ -1481,7 +1461,7 @@
       <c r="C48" s="15"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>29</v>
       </c>
@@ -1491,7 +1471,7 @@
       <c r="C49" s="11"/>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>31</v>
       </c>
@@ -1505,7 +1485,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>32</v>
       </c>
@@ -1517,7 +1497,7 @@
       </c>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>33</v>
       </c>
@@ -1529,7 +1509,7 @@
       </c>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>34</v>
       </c>
@@ -1541,7 +1521,7 @@
       </c>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>35</v>
       </c>
@@ -1553,7 +1533,7 @@
       </c>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>36</v>
       </c>
@@ -1565,7 +1545,7 @@
       </c>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>37</v>
       </c>
@@ -1576,10 +1556,10 @@
         <v>0</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>88</v>
       </c>
@@ -1591,7 +1571,7 @@
       </c>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>89</v>
       </c>
@@ -1600,10 +1580,10 @@
       </c>
       <c r="C58" s="17"/>
       <c r="D58" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>90</v>
       </c>
@@ -1615,7 +1595,7 @@
       </c>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>97</v>
       </c>
@@ -1624,10 +1604,10 @@
       </c>
       <c r="C60" s="17"/>
       <c r="D60" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>116</v>
       </c>
@@ -1635,7 +1615,7 @@
       <c r="C61" s="15"/>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>117</v>
       </c>
@@ -1643,12 +1623,12 @@
       <c r="C62" s="15"/>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="7"/>
       <c r="B63" s="8"/>
       <c r="C63" s="10">
         <f>AVERAGE(C2:C62)</f>
-        <v>0.85384615384615381</v>
+        <v>0.87307692307692308</v>
       </c>
       <c r="D63" s="8"/>
     </row>
@@ -1668,7 +1648,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1680,7 +1660,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed incorrect operations of the scrollbars.
</commit_message>
<xml_diff>
--- a/dev_info/gk_linux_mono_compatibility_ru.xlsx
+++ b/dev_info/gk_linux_mono_compatibility_ru.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
   <si>
     <t>Базовый функционал</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Работа основных списков записей (ListView)</t>
   </si>
   <si>
-    <t>Странный скроллинг</t>
-  </si>
-  <si>
     <t>1.1.2</t>
   </si>
   <si>
@@ -262,9 +259,6 @@
   </si>
   <si>
     <t>Отправка логов почтой</t>
-  </si>
-  <si>
-    <t>Странный скроллинг и отображение</t>
   </si>
   <si>
     <t>Не работает WebBrowser</t>
@@ -866,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -879,13 +873,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>20</v>
@@ -924,15 +918,15 @@
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="C5" s="12">
         <v>1</v>
@@ -941,10 +935,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="C6" s="12">
         <v>1</v>
@@ -1042,19 +1036,17 @@
       <c r="B14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="14">
-        <v>0.75</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="C14" s="12">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="12">
         <v>1</v>
@@ -1066,7 +1058,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="12">
         <v>1</v>
@@ -1078,7 +1070,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="12">
         <v>1</v>
@@ -1090,21 +1082,19 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="14">
-        <v>0.75</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>42</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C18" s="12">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="12">
         <v>1</v>
@@ -1116,13 +1106,13 @@
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20" s="14">
         <v>0.5</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1130,35 +1120,35 @@
         <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" s="13">
         <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C22" s="13">
         <v>0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23" s="12">
         <v>1</v>
@@ -1167,10 +1157,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" s="12">
         <v>1</v>
@@ -1179,38 +1169,36 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="14">
-        <v>0.75</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>42</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C25" s="12">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C26" s="13">
         <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C27" s="12">
         <v>1</v>
@@ -1219,10 +1207,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C28" s="12">
         <v>1</v>
@@ -1231,10 +1219,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" s="12">
         <v>1</v>
@@ -1243,10 +1231,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C30" s="12">
         <v>1</v>
@@ -1255,10 +1243,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" s="12">
         <v>1</v>
@@ -1267,10 +1255,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C32" s="12">
         <v>1</v>
@@ -1279,10 +1267,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="12">
         <v>1</v>
@@ -1291,10 +1279,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C34" s="12">
         <v>1</v>
@@ -1303,10 +1291,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C35" s="12">
         <v>1</v>
@@ -1315,7 +1303,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="15"/>
@@ -1333,10 +1321,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="C38" s="12">
         <v>1</v>
@@ -1345,10 +1333,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C39" s="12">
         <v>1</v>
@@ -1357,10 +1345,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C40" s="12">
         <v>1</v>
@@ -1369,10 +1357,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C41" s="12">
         <v>1</v>
@@ -1381,10 +1369,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C42" s="12">
         <v>1</v>
@@ -1393,10 +1381,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C43" s="12">
         <v>1</v>
@@ -1405,10 +1393,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C44" s="12">
         <v>1</v>
@@ -1417,10 +1405,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C45" s="12">
         <v>1</v>
@@ -1429,24 +1417,24 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C46" s="14">
         <v>0.75</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C47" s="12">
         <v>1</v>
@@ -1455,7 +1443,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="15"/>
@@ -1476,13 +1464,13 @@
         <v>31</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C50" s="16">
         <v>0.9</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1490,7 +1478,7 @@
         <v>32</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C51" s="12">
         <v>1</v>
@@ -1502,7 +1490,7 @@
         <v>33</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C52" s="12">
         <v>1</v>
@@ -1514,7 +1502,7 @@
         <v>34</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C53" s="12">
         <v>1</v>
@@ -1526,7 +1514,7 @@
         <v>35</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C54" s="12">
         <v>1</v>
@@ -1538,7 +1526,7 @@
         <v>36</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C55" s="12">
         <v>1</v>
@@ -1550,21 +1538,21 @@
         <v>37</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C56" s="13">
         <v>0</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C57" s="12">
         <v>1</v>
@@ -1573,22 +1561,22 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C58" s="17"/>
       <c r="D58" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C59" s="12">
         <v>1</v>
@@ -1597,19 +1585,19 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C60" s="17"/>
       <c r="D60" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="15"/>
@@ -1617,7 +1605,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="15"/>
@@ -1628,7 +1616,7 @@
       <c r="B63" s="8"/>
       <c r="C63" s="10">
         <f>AVERAGE(C2:C62)</f>
-        <v>0.87307692307692308</v>
+        <v>0.88749999999999996</v>
       </c>
       <c r="D63" s="8"/>
     </row>

</xml_diff>

<commit_message>
Fixed work of SingleInstance in Linux
</commit_message>
<xml_diff>
--- a/dev_info/gk_linux_mono_compatibility_ru.xlsx
+++ b/dev_info/gk_linux_mono_compatibility_ru.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="130">
   <si>
     <t>Базовый функционал</t>
   </si>
@@ -384,9 +384,6 @@
     <t>Просмотр графа связей</t>
   </si>
   <si>
-    <t>SingleInstance не работает (Main)</t>
-  </si>
-  <si>
     <t>1.31</t>
   </si>
   <si>
@@ -397,9 +394,6 @@
   </si>
   <si>
     <t>Не формируется PDF (iTextSharp), dll-depend</t>
-  </si>
-  <si>
-    <t>Только генерация и просмотр HTML, не формируется PDF (iTextSharp), dll-depend</t>
   </si>
   <si>
     <t>ArborGVT подвисает</t>
@@ -861,14 +855,14 @@
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="81.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -914,12 +908,10 @@
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="13">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>122</v>
-      </c>
+      <c r="C4" s="12">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1112,7 +1104,7 @@
         <v>0.5</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1126,7 +1118,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1190,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1294,7 +1286,7 @@
         <v>77</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C35" s="12">
         <v>1</v>
@@ -1303,7 +1295,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="15"/>
@@ -1426,7 +1418,7 @@
         <v>0.75</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1544,7 +1536,7 @@
         <v>0</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1568,7 +1560,7 @@
       </c>
       <c r="C58" s="17"/>
       <c r="D58" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1592,7 +1584,7 @@
       </c>
       <c r="C60" s="17"/>
       <c r="D60" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1616,7 +1608,7 @@
       <c r="B63" s="8"/>
       <c r="C63" s="10">
         <f>AVERAGE(C2:C62)</f>
-        <v>0.88749999999999996</v>
+        <v>0.90673076923076923</v>
       </c>
       <c r="D63" s="8"/>
     </row>

</xml_diff>